<commit_message>
Updated PhantomJs code and Chrome Headless
</commit_message>
<xml_diff>
--- a/ExcelSheets/REMIT/TC_Remit.xlsx
+++ b/ExcelSheets/REMIT/TC_Remit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="200" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="990" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId2" sheetId="1" state="visible"/>
@@ -13,321 +13,398 @@
     <sheet name="Data" r:id="rId4" sheetId="3" state="visible"/>
   </sheets>
   <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="119">
-  <si>
-    <t>TCID</t>
-  </si>
-  <si>
-    <t>RunMode</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>TC_Login</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Validate the user Login into the System</t>
-  </si>
-  <si>
-    <t>TC_AddNewSender</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Validate a New Sender can be added</t>
-  </si>
-  <si>
-    <t>TC_ExistingSender</t>
-  </si>
-  <si>
-    <t>Verify the existing Sender</t>
-  </si>
-  <si>
-    <t>TC_AddBeneficiaryDetails</t>
-  </si>
-  <si>
-    <t>Check the beneficiary can be added</t>
-  </si>
-  <si>
-    <t>TC_TransferMoney</t>
-  </si>
-  <si>
-    <t>Validate the money can be transferred</t>
-  </si>
-  <si>
-    <t>TC_SenderAmount</t>
-  </si>
-  <si>
-    <t>Checking the Balance of the sender</t>
-  </si>
-  <si>
-    <t>TC_ValidateTransfer</t>
-  </si>
-  <si>
-    <t>Validating the Transfer Held</t>
-  </si>
-  <si>
-    <t>TC_DeleteBeneficary</t>
-  </si>
-  <si>
-    <t>Deleting the Beneficiary holder</t>
-  </si>
-  <si>
-    <t>Keywords</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>openBrowser</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>navigateTo</t>
-  </si>
-  <si>
-    <t>Live_url</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>username_id</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>password_id</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>loginButton_xpath</t>
-  </si>
-  <si>
-    <t>loginOtp</t>
-  </si>
-  <si>
-    <t>verifyText</t>
-  </si>
-  <si>
-    <t>UserId_xpath</t>
-  </si>
-  <si>
-    <t>Expected text</t>
-  </si>
-  <si>
-    <t>GetText</t>
-  </si>
-  <si>
-    <t>Userbal_xpath</t>
-  </si>
-  <si>
-    <t>closeBrowser</t>
-  </si>
-  <si>
-    <t>getLogin</t>
-  </si>
-  <si>
-    <t>add_searchNumber_id</t>
-  </si>
-  <si>
-    <t>Add/Search</t>
-  </si>
-  <si>
-    <t>existName_xpath</t>
-  </si>
-  <si>
-    <t>existBalance_xpath</t>
-  </si>
-  <si>
-    <t>takeScreenShot</t>
-  </si>
-  <si>
-    <t>INFO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="135">
+  <si>
+    <t xml:space="preserve">TCID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RunMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the user Login into the System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_AddNewSender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate a New Sender can be added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_ExistingSender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the existing Sender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_AddBeneficiaryDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the beneficiary can be added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_TransferMoney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the money can be transferred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_SenderAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checking the Balance of the sender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_ValidateTransfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating the Transfer Held</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_DeleteBeneficary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deleting the Beneficiary holder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keywords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openBrowser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully created a instance of chrome PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigateTo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Live_url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully navigated to Live_url PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entered Value in the Field PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loginButton_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicked on loginButton_xpath PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loginOtp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO Otp Panel Displayed FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verifyText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserId_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text is verified PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GetText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Userbal_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully Fetched the value PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closeBrowser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getLogin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_searchNumber_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add/Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existName_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existBalance_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">takeScreenShot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addSender_Name_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SenderName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addOtpNumber_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addSenderConfirmBtn_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO Otp Panel Displayed FAILPASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waited for 20 sec PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beneficaryAddBtn_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicked on beneficaryAddBtn_xpath PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchBank_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BankName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icicBnk_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicked on icicBnk_xpath PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beneficiaryAccountNum_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccountNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beneficiaryPhoneNum_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhoneNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addBeneficiaryBtn_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicked on addBeneficiaryBtn_xpath PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unable to take the screenshot FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text is not verified FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error While entering the Values ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstradio_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transactionamount_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transferBtn_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report_url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orderId_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deleteBen_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getAlertText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AcceptAlert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9819042543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Anand 123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test got Successfully Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExpectedResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7101001212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajinkya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9967903705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">195905000005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t>Successfully created a instance of chrome PASS</t>
+  </si>
+  <si>
+    <t>Successfully navigated to Live_url PASS</t>
+  </si>
+  <si>
+    <t>NO Otp Panel Displayed FAILPASS</t>
+  </si>
+  <si>
+    <t>Waited for 20 sec PASS</t>
+  </si>
+  <si>
+    <t>Text is verified PASS</t>
+  </si>
+  <si>
+    <t>Entered Value in the Field PASS</t>
+  </si>
+  <si>
+    <t>Clicked on firstradio_xpath PASS</t>
+  </si>
+  <si>
+    <t>Clicked on transferBtn_id PASS</t>
   </si>
   <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>wait</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>addSender_Name_id</t>
-  </si>
-  <si>
-    <t>SenderName</t>
-  </si>
-  <si>
-    <t>Otp</t>
-  </si>
-  <si>
-    <t>addOtpNumber_id</t>
-  </si>
-  <si>
-    <t>addSenderConfirmBtn_xpath</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>beneficaryAddBtn_xpath</t>
-  </si>
-  <si>
-    <t>searchBank_id</t>
-  </si>
-  <si>
-    <t>BankName</t>
-  </si>
-  <si>
-    <t>icicBnk_xpath</t>
-  </si>
-  <si>
-    <t>beneficiaryAccountNum_id</t>
-  </si>
-  <si>
-    <t>AccountNum</t>
-  </si>
-  <si>
-    <t>beneficiaryPhoneNum_id</t>
-  </si>
-  <si>
-    <t>PhoneNo</t>
-  </si>
-  <si>
-    <t>addBeneficiaryBtn_xpath</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
-    <t>firstradio_xpath</t>
-  </si>
-  <si>
-    <t>transactionamount_id</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>transferBtn_id</t>
-  </si>
-  <si>
-    <t>8000</t>
-  </si>
-  <si>
-    <t>report_url</t>
-  </si>
-  <si>
-    <t>orderId_xpath</t>
-  </si>
-  <si>
-    <t>deleteBen_xpath</t>
-  </si>
-  <si>
-    <t>getAlertText</t>
-  </si>
-  <si>
-    <t>AcceptAlert</t>
-  </si>
-  <si>
-    <t>Accept</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Actual Result</t>
-  </si>
-  <si>
-    <t>Mozilla</t>
-  </si>
-  <si>
-    <t>9819042543</t>
-  </si>
-  <si>
-    <t>1234567</t>
-  </si>
-  <si>
-    <t>Test Anand 123</t>
-  </si>
-  <si>
-    <t>ExpectedResult</t>
-  </si>
-  <si>
-    <t>7101001212</t>
-  </si>
-  <si>
-    <t>Ajinkya</t>
+    <t>Pass</t>
   </si>
   <si>
     <t>Test got Successfully Passed</t>
   </si>
   <si>
-    <t>9967903705</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>ICIC</t>
-  </si>
-  <si>
-    <t>195905000005</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>Skip</t>
   </si>
   <si>
-    <t>Successfully created a instance of Mozilla PASS</t>
-  </si>
-  <si>
-    <t>Successfully navigated to Live_url PASS</t>
-  </si>
-  <si>
-    <t>NO Otp Panel Displayed FAILPASS</t>
-  </si>
-  <si>
-    <t>Text is verified PASS</t>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Error While entering the Values ERROR</t>
+  </si>
+  <si>
+    <t>Clicked on loginButton_xpath PASS</t>
+  </si>
+  <si>
+    <t>NO Otp Panel Displayed FAIL</t>
   </si>
   <si>
     <t>Successfully Fetched the value PASS</t>
   </si>
   <si>
-    <t>Entered Value in the Field PASS</t>
-  </si>
-  <si>
-    <t>Waited for 20 sec PASS</t>
-  </si>
-  <si>
     <t>Clicked on beneficaryAddBtn_xpath PASS</t>
   </si>
   <si>
@@ -337,27 +414,6 @@
     <t>Clicked on addBeneficiaryBtn_xpath PASS</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Failed to excute the test</t>
-  </si>
-  <si>
-    <t>Clicked on loginButton_xpath PASS</t>
-  </si>
-  <si>
-    <t>NO Otp Panel Displayed FAIL</t>
-  </si>
-  <si>
-    <t>Clicked on firstradio_xpath PASS</t>
-  </si>
-  <si>
-    <t>Clicked on transferBtn_id PASS</t>
-  </si>
-  <si>
     <t>Successfully navigated to report_url PASS</t>
   </si>
   <si>
@@ -370,10 +426,7 @@
     <t>Accepting the Alert Option PASS</t>
   </si>
   <si>
-    <t>Caught in CatchLive_urlFAIL</t>
-  </si>
-  <si>
-    <t>Unable to launch browserFAIL</t>
+    <t>Text is not verified FAIL</t>
   </si>
 </sst>
 </file>
@@ -381,7 +434,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -528,7 +581,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="364">
+  <cellXfs count="280">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -545,38 +598,46 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="7" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -624,264 +685,6 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="true"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="true"/>
@@ -1730,11 +1533,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="1" width="25.4234693877551" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="1" width="11.5204081632653" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="1" width="50.3418367346939" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="1" width="24.8367346938776" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="1" width="49.1377551020408" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" hidden="false" style="1" width="7.60546875" collapsed="true"/>
-    <col min="5" max="1025" hidden="false" style="1" width="11.5204081632653" collapsed="true"/>
+    <col min="5" max="1025" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="1">
@@ -1761,8 +1564,8 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="310" t="s">
-        <v>91</v>
+      <c r="D2" s="241" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="3">
@@ -1775,8 +1578,8 @@
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="358" t="s">
-        <v>95</v>
+      <c r="D3" s="270" t="s">
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="4">
@@ -1789,8 +1592,8 @@
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="276" t="s">
-        <v>91</v>
+      <c r="D4" s="227" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="5">
@@ -1803,8 +1606,8 @@
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="363" t="s">
-        <v>107</v>
+      <c r="D5" s="277" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
@@ -1817,8 +1620,8 @@
       <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="326" t="s">
-        <v>91</v>
+      <c r="D6" s="246" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="7">
@@ -1831,8 +1634,8 @@
       <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="287" t="s">
-        <v>91</v>
+      <c r="D7" s="232" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="8">
@@ -1845,8 +1648,8 @@
       <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="336" t="s">
-        <v>91</v>
+      <c r="D8" s="251" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="9">
@@ -1859,8 +1662,8 @@
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="350" t="s">
-        <v>91</v>
+      <c r="D9" s="256" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1882,17 +1685,17 @@
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B15" activeCellId="0" pane="topLeft" sqref="B15"/>
+      <selection activeCell="D103" activeCellId="0" pane="topLeft" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="7" width="32.5051020408163" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="7" width="22.6428571428571" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="7" width="31.8112244897959" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="7" width="21.5357142857143" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" hidden="false" style="7" width="40.46875" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="7" width="11.5204081632653" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="7" width="31.7244897959184" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="7" width="22.0051020408163" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="7" width="31.0459183673469" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="7" width="21.0612244897959" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" hidden="false" style="7" width="41.0546875" collapsed="true"/>
+    <col min="6" max="1025" hidden="false" style="7" width="11.0714285714286" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="1">
@@ -1923,8 +1726,8 @@
       <c r="D2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="299" t="s">
-        <v>96</v>
+      <c r="E2" s="233" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="3">
@@ -1932,14 +1735,14 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="9"/>
-      <c r="E3" s="300" t="s">
-        <v>97</v>
+      <c r="E3" s="234" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="4">
@@ -1947,16 +1750,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="301" t="s">
-        <v>101</v>
+        <v>33</v>
+      </c>
+      <c r="E4" s="235" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="5">
@@ -1964,16 +1767,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="302" t="s">
-        <v>101</v>
+        <v>36</v>
+      </c>
+      <c r="E5" s="236" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
@@ -1981,14 +1784,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="303" t="s">
-        <v>109</v>
+      <c r="E6" s="237" t="s">
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="7">
@@ -1996,12 +1799,12 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="304" t="s">
-        <v>110</v>
+      <c r="E7" s="238" t="s">
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="8">
@@ -2009,16 +1812,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="305" t="s">
-        <v>99</v>
+        <v>44</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="9">
@@ -2026,14 +1829,14 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="306" t="s">
-        <v>100</v>
+      <c r="E9" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="10">
@@ -2041,11 +1844,11 @@
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="307" t="s">
+      <c r="E10" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2060,8 +1863,8 @@
       <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="266" t="s">
-        <v>96</v>
+      <c r="E11" s="278" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="12">
@@ -2069,14 +1872,14 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="267" t="s">
-        <v>97</v>
+      <c r="E12" s="279" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="13">
@@ -2084,12 +1887,12 @@
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="268" t="s">
-        <v>98</v>
+      <c r="E13" s="148" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="14">
@@ -2097,16 +1900,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="269" t="s">
-        <v>99</v>
+        <v>43</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="149" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="15">
@@ -2114,16 +1917,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="270" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="E15" s="150" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="16">
@@ -2131,14 +1934,14 @@
         <v>10</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="271" t="s">
-        <v>100</v>
+      <c r="E16" s="151" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="17">
@@ -2146,14 +1949,14 @@
         <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="272" t="s">
-        <v>100</v>
+      <c r="E17" s="152" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
@@ -2161,25 +1964,25 @@
         <v>10</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="19">
       <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="273" t="s">
-        <v>50</v>
+      <c r="E19" s="153" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="20">
@@ -2187,7 +1990,7 @@
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
       <c r="A21" s="6" t="s">
@@ -2200,185 +2003,185 @@
       <c r="D21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="23">
       <c r="A23" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="24">
       <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="E24" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="25">
       <c r="A25" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="26">
       <c r="A26" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="E26" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="27">
       <c r="A27" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D27" s="9"/>
-      <c r="E27" s="4"/>
+      <c r="E27" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="28">
       <c r="A28" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="E28" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="29">
       <c r="A29" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D29" s="9"/>
-      <c r="E29" s="4"/>
+      <c r="E29" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="30">
       <c r="A30" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D30" s="9"/>
-      <c r="E30" s="4"/>
+      <c r="E30" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="31">
       <c r="A31" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D31" s="9"/>
-      <c r="E31" s="4"/>
+      <c r="E31" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="32">
       <c r="A32" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D32" s="9"/>
-      <c r="E32" s="4"/>
+      <c r="E32" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="33">
       <c r="A33" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D33" s="9"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="34">
       <c r="A34" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="35">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="36">
       <c r="A36" s="6" t="s">
@@ -2391,8 +2194,8 @@
       <c r="D36" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="359" t="s">
-        <v>118</v>
+      <c r="E36" s="271" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="37">
@@ -2400,14 +2203,14 @@
         <v>12</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D37" s="9"/>
-      <c r="E37" s="360" t="s">
-        <v>117</v>
+      <c r="E37" s="272" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="38">
@@ -2415,12 +2218,12 @@
         <v>12</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="9"/>
-      <c r="E38" s="245" t="s">
-        <v>98</v>
+      <c r="E38" s="273" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="39">
@@ -2428,16 +2231,16 @@
         <v>12</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" s="246" t="s">
-        <v>99</v>
+        <v>44</v>
+      </c>
+      <c r="E39" s="274" t="s">
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="40">
@@ -2445,14 +2248,14 @@
         <v>12</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D40" s="9"/>
-      <c r="E40" s="247" t="s">
-        <v>100</v>
+      <c r="E40" s="127" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="41">
@@ -2460,14 +2263,14 @@
         <v>12</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D41" s="9"/>
-      <c r="E41" s="248" t="s">
-        <v>50</v>
+      <c r="E41" s="128" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="42">
@@ -2475,16 +2278,16 @@
         <v>12</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E42" s="249" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="E42" s="129" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="43">
@@ -2492,14 +2295,14 @@
         <v>12</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D43" s="9"/>
-      <c r="E43" s="250" t="s">
-        <v>102</v>
+      <c r="E43" s="130" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="44">
@@ -2507,14 +2310,14 @@
         <v>12</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D44" s="9"/>
-      <c r="E44" s="251" t="s">
-        <v>100</v>
+      <c r="E44" s="131" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="45">
@@ -2522,14 +2325,14 @@
         <v>12</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D45" s="9"/>
-      <c r="E45" s="252" t="s">
-        <v>100</v>
+      <c r="E45" s="132" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="46">
@@ -2537,27 +2340,27 @@
         <v>12</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D46" s="9"/>
-      <c r="E46" s="4"/>
+      <c r="E46" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="47">
       <c r="A47" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D47" s="9"/>
-      <c r="E47" s="253" t="s">
-        <v>103</v>
+      <c r="E47" s="133" t="s">
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="48">
@@ -2565,14 +2368,14 @@
         <v>12</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D48" s="9"/>
-      <c r="E48" s="254" t="s">
-        <v>102</v>
+      <c r="E48" s="134" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="49">
@@ -2580,16 +2383,16 @@
         <v>12</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="255" t="s">
-        <v>101</v>
+        <v>70</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" s="135" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="50">
@@ -2597,14 +2400,14 @@
         <v>12</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D50" s="9"/>
-      <c r="E50" s="256" t="s">
-        <v>104</v>
+      <c r="E50" s="136" t="s">
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="51">
@@ -2612,14 +2415,14 @@
         <v>12</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D51" s="9"/>
-      <c r="E51" s="257" t="s">
-        <v>102</v>
+      <c r="E51" s="137" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="52">
@@ -2627,16 +2430,16 @@
         <v>12</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E52" s="258" t="s">
-        <v>101</v>
+        <v>75</v>
+      </c>
+      <c r="E52" s="138" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="53">
@@ -2644,16 +2447,16 @@
         <v>12</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E53" s="259" t="s">
-        <v>101</v>
+        <v>77</v>
+      </c>
+      <c r="E53" s="139" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="54">
@@ -2661,14 +2464,14 @@
         <v>12</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D54" s="6"/>
-      <c r="E54" s="260" t="s">
-        <v>105</v>
+      <c r="E54" s="140" t="s">
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="55">
@@ -2676,14 +2479,14 @@
         <v>12</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D55" s="6"/>
-      <c r="E55" s="261" t="s">
-        <v>102</v>
+      <c r="E55" s="141" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="56">
@@ -2691,25 +2494,27 @@
         <v>12</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D56" s="6"/>
-      <c r="E56" s="4"/>
+      <c r="E56" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="57">
       <c r="A57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
-      <c r="E57" s="262" t="s">
-        <v>106</v>
+      <c r="E57" s="142" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="58">
@@ -2723,8 +2528,8 @@
       <c r="D58" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="277" t="s">
-        <v>96</v>
+      <c r="E58" s="228" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="59">
@@ -2732,14 +2537,14 @@
         <v>16</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D59" s="6"/>
-      <c r="E59" s="278" t="s">
-        <v>97</v>
+      <c r="E59" s="229" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="60">
@@ -2747,12 +2552,12 @@
         <v>16</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
-      <c r="E60" s="279" t="s">
-        <v>98</v>
+      <c r="E60" s="159" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="61">
@@ -2760,16 +2565,16 @@
         <v>16</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E61" s="280" t="s">
-        <v>99</v>
+        <v>44</v>
+      </c>
+      <c r="E61" s="160" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="62">
@@ -2777,16 +2582,16 @@
         <v>16</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" s="281" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="E62" s="161" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="63">
@@ -2794,14 +2599,14 @@
         <v>16</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D63" s="6"/>
-      <c r="E63" s="282" t="s">
-        <v>100</v>
+      <c r="E63" s="162" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="64">
@@ -2809,14 +2614,14 @@
         <v>16</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D64" s="6"/>
-      <c r="E64" s="283" t="s">
-        <v>100</v>
+      <c r="E64" s="163" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="65">
@@ -2824,25 +2629,25 @@
         <v>16</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D65" s="6"/>
-      <c r="E65" s="4"/>
+      <c r="E65" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="66">
       <c r="A66" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
-      <c r="E66" s="284" t="s">
-        <v>50</v>
+      <c r="E66" s="164" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="67">
@@ -2856,8 +2661,8 @@
       <c r="D67" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E67" s="311" t="s">
-        <v>96</v>
+      <c r="E67" s="242" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="68">
@@ -2865,14 +2670,14 @@
         <v>14</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D68" s="9"/>
-      <c r="E68" s="312" t="s">
-        <v>97</v>
+      <c r="E68" s="243" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="69">
@@ -2880,12 +2685,12 @@
         <v>14</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="9"/>
-      <c r="E69" s="313" t="s">
-        <v>98</v>
+      <c r="E69" s="179" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="70">
@@ -2893,14 +2698,14 @@
         <v>14</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D70" s="9"/>
-      <c r="E70" s="314" t="s">
-        <v>102</v>
+      <c r="E70" s="180" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="71">
@@ -2908,16 +2713,16 @@
         <v>14</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E71" s="315" t="s">
-        <v>99</v>
+        <v>44</v>
+      </c>
+      <c r="E71" s="181" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="72">
@@ -2925,16 +2730,16 @@
         <v>14</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E72" s="316" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="E72" s="182" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="73">
@@ -2942,14 +2747,14 @@
         <v>14</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D73" s="6"/>
-      <c r="E73" s="317" t="s">
-        <v>111</v>
+      <c r="E73" s="183" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="74">
@@ -2957,16 +2762,16 @@
         <v>14</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E74" s="318" t="s">
-        <v>101</v>
+        <v>86</v>
+      </c>
+      <c r="E74" s="184" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="75">
@@ -2974,14 +2779,14 @@
         <v>14</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D75" s="6"/>
-      <c r="E75" s="319" t="s">
-        <v>102</v>
+      <c r="E75" s="185" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="76">
@@ -2989,27 +2794,27 @@
         <v>14</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D76" s="6"/>
-      <c r="E76" s="4"/>
+      <c r="E76" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="77">
       <c r="A77" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D77" s="6"/>
-      <c r="E77" s="320" t="s">
-        <v>112</v>
+      <c r="E77" s="186" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="78">
@@ -3017,14 +2822,14 @@
         <v>14</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D78" s="6"/>
-      <c r="E78" s="321" t="s">
-        <v>102</v>
+      <c r="E78" s="187" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="79">
@@ -3032,14 +2837,14 @@
         <v>14</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D79" s="6"/>
-      <c r="E79" s="322" t="s">
-        <v>50</v>
+      <c r="E79" s="188" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="80">
@@ -3047,12 +2852,12 @@
         <v>14</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
-      <c r="E80" s="323" t="s">
-        <v>50</v>
+      <c r="E80" s="189" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="81">
@@ -3066,8 +2871,8 @@
       <c r="D81" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E81" s="327" t="s">
-        <v>96</v>
+      <c r="E81" s="247" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="82">
@@ -3075,14 +2880,14 @@
         <v>18</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D82" s="9"/>
-      <c r="E82" s="328" t="s">
-        <v>97</v>
+      <c r="E82" s="248" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="83">
@@ -3090,12 +2895,12 @@
         <v>18</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
-      <c r="E83" s="329" t="s">
-        <v>98</v>
+      <c r="E83" s="195" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="84">
@@ -3103,16 +2908,16 @@
         <v>18</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E84" s="330" t="s">
-        <v>99</v>
+        <v>44</v>
+      </c>
+      <c r="E84" s="196" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="85">
@@ -3120,14 +2925,14 @@
         <v>18</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D85" s="6"/>
-      <c r="E85" s="331" t="s">
-        <v>113</v>
+      <c r="E85" s="197" t="s">
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="86">
@@ -3135,16 +2940,16 @@
         <v>18</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C86" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E86" s="332" t="s">
-        <v>99</v>
+      <c r="E86" s="198" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="87">
@@ -3152,25 +2957,25 @@
         <v>18</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D87" s="6"/>
-      <c r="E87" s="4"/>
+      <c r="E87" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="88">
       <c r="A88" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
-      <c r="E88" s="333" t="s">
-        <v>50</v>
+      <c r="E88" s="199" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="89">
@@ -3184,8 +2989,8 @@
       <c r="D89" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E89" s="337" t="s">
-        <v>96</v>
+      <c r="E89" s="252" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="90">
@@ -3193,14 +2998,14 @@
         <v>20</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D90" s="9"/>
-      <c r="E90" s="338" t="s">
-        <v>97</v>
+      <c r="E90" s="253" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="91">
@@ -3208,12 +3013,12 @@
         <v>20</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
-      <c r="E91" s="339" t="s">
-        <v>98</v>
+      <c r="E91" s="205" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="92">
@@ -3221,16 +3026,16 @@
         <v>20</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E92" s="340" t="s">
-        <v>99</v>
+        <v>44</v>
+      </c>
+      <c r="E92" s="206" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="93">
@@ -3238,16 +3043,16 @@
         <v>20</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E93" s="341" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="E93" s="207" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="94">
@@ -3255,13 +3060,13 @@
         <v>20</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E94" s="342" t="s">
-        <v>111</v>
+        <v>84</v>
+      </c>
+      <c r="E94" s="208" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="95">
@@ -3269,13 +3074,13 @@
         <v>20</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E95" s="343" t="s">
-        <v>114</v>
+        <v>91</v>
+      </c>
+      <c r="E95" s="209" t="s">
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="96">
@@ -3283,13 +3088,13 @@
         <v>20</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E96" s="344" t="s">
-        <v>102</v>
+        <v>59</v>
+      </c>
+      <c r="E96" s="210" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="97">
@@ -3297,11 +3102,11 @@
         <v>20</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C97" s="0"/>
-      <c r="E97" s="345" t="s">
-        <v>115</v>
+      <c r="E97" s="211" t="s">
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="98">
@@ -3309,13 +3114,13 @@
         <v>20</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C98" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E98" s="346" t="s">
-        <v>116</v>
+        <v>93</v>
+      </c>
+      <c r="C98" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E98" s="212" t="s">
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="99">
@@ -3323,10 +3128,10 @@
         <v>20</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E99" s="347" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="E99" s="213" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3347,29 +3152,29 @@
   </sheetPr>
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G3" activeCellId="0" pane="topLeft" sqref="G3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="I13" activeCellId="0" pane="topLeft" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" hidden="false" style="1" width="27.47265625" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="1" width="11.5204081632653" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="1" width="14.0765306122449" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="1" width="11.5714285714286" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="1" width="22.8316326530612" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="1" width="20.3316326530612" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" hidden="false" style="1" width="24.9453125" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="1" width="27.1326530612245" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="1" width="13.6326530612245" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="1" width="22.2755102040816" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="1" width="19.7091836734694" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" hidden="false" style="1" width="15.33203125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" hidden="false" style="1" width="12.01953125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" hidden="false" style="1" width="12.01953125" collapsed="true"/>
-    <col min="10" max="10" hidden="false" style="1" width="14.2295918367347" collapsed="true"/>
-    <col min="11" max="11" hidden="false" style="1" width="14.0765306122449" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="1" width="13.7704081632653" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="1" width="13.6326530612245" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" hidden="false" style="1" width="6.171875" collapsed="true"/>
-    <col min="13" max="1025" hidden="false" style="1" width="11.5204081632653" collapsed="true"/>
+    <col min="13" max="1025" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="10"/>
@@ -3385,28 +3190,28 @@
       <c r="L1" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="19" t="s">
+      <c r="D2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="10"/>
@@ -3415,57 +3220,41 @@
       <c r="L2" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="298" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="297" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" s="4"/>
+      <c r="G3" s="240"/>
+      <c r="H3" s="239" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" s="13"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>85</v>
-      </c>
+      <c r="A4" s="13"/>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="309" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" s="308" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="13"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="0"/>
@@ -3485,7 +3274,7 @@
       <c r="L5" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="10"/>
@@ -3501,64 +3290,64 @@
       <c r="L6" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="19" t="s">
+      <c r="D7" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="21" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="13"/>
       <c r="H8" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" s="4"/>
+        <v>105</v>
+      </c>
+      <c r="J8" s="13"/>
       <c r="K8" s="10"/>
       <c r="L8" s="0"/>
     </row>
@@ -3591,7 +3380,7 @@
       <c r="L10" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="11">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="10"/>
@@ -3607,31 +3396,31 @@
       <c r="L11" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="12">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="19" t="s">
+      <c r="D12" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="21" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="10"/>
@@ -3643,26 +3432,24 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="275" t="s">
-        <v>89</v>
-      </c>
+      <c r="G13" s="226"/>
       <c r="H13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I13" s="274" t="s">
-        <v>91</v>
+        <v>106</v>
+      </c>
+      <c r="I13" s="225" t="s">
+        <v>122</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -3697,7 +3484,7 @@
       <c r="L15" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="16">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="10"/>
@@ -3713,73 +3500,75 @@
       <c r="L16" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="17">
-      <c r="A17" s="362"/>
-      <c r="B17" s="20" t="s">
+      <c r="A17" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="20" t="s">
+      <c r="C17" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G17" s="355"/>
-      <c r="H17" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="L17" s="354" t="s">
+      <c r="D17" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="0"/>
+      <c r="G18" s="276"/>
+      <c r="H18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
-      <c r="A18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="0"/>
-      <c r="G18" s="264" t="s">
+      <c r="J18" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="K18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L18" s="263" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="L18" s="275" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="19">
@@ -3809,7 +3598,7 @@
       <c r="K20" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="24" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="0"/>
@@ -3824,66 +3613,64 @@
       <c r="K21" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="22">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="20" t="s">
+      <c r="C22" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="18" t="s">
+      <c r="D22" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="K22" s="21"/>
+      <c r="K22" s="23"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="23">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F23" s="0"/>
-      <c r="G23" s="325" t="s">
-        <v>89</v>
-      </c>
+      <c r="G23" s="245"/>
       <c r="H23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I23" s="324" t="s">
-        <v>91</v>
+        <v>106</v>
+      </c>
+      <c r="I23" s="244" t="s">
+        <v>122</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="24">
@@ -3899,7 +3686,7 @@
       <c r="J24" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="0"/>
@@ -3913,31 +3700,31 @@
       <c r="J25" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="26">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="20" t="s">
+      <c r="C26" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I26" s="19" t="s">
+      <c r="D26" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" s="21" t="s">
         <v>3</v>
       </c>
       <c r="J26" s="0"/>
@@ -3947,26 +3734,24 @@
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F27" s="10"/>
-      <c r="G27" s="286" t="s">
-        <v>89</v>
-      </c>
+      <c r="G27" s="231"/>
       <c r="H27" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I27" s="285" t="s">
-        <v>91</v>
+        <v>106</v>
+      </c>
+      <c r="I27" s="230" t="s">
+        <v>122</v>
       </c>
       <c r="J27" s="0"/>
     </row>
@@ -3995,7 +3780,7 @@
       <c r="J29" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="30">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B30" s="0"/>
@@ -4009,35 +3794,35 @@
       <c r="J30" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="31">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="20" t="s">
+      <c r="C31" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H31" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I31" s="19" t="s">
+      <c r="D31" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="21" t="s">
-        <v>64</v>
+      <c r="J31" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="32">
@@ -4045,29 +3830,27 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F32" s="10"/>
-      <c r="G32" s="335" t="s">
-        <v>89</v>
-      </c>
+      <c r="G32" s="250"/>
       <c r="H32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I32" s="334" t="s">
-        <v>91</v>
+        <v>106</v>
+      </c>
+      <c r="I32" s="249" t="s">
+        <v>122</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="33">
@@ -4093,7 +3876,7 @@
       <c r="I34" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="35">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="0"/>
@@ -4106,32 +3889,32 @@
       <c r="I35" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="36">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="20" t="s">
+      <c r="C36" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H36" s="1" t="s">
+      <c r="D36" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I36" s="21" t="s">
-        <v>45</v>
+      <c r="I36" s="23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="37">
@@ -4139,26 +3922,24 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F37" s="10"/>
-      <c r="G37" s="349" t="s">
-        <v>89</v>
-      </c>
-      <c r="H37" s="348" t="s">
-        <v>91</v>
+      <c r="G37" s="255"/>
+      <c r="H37" s="254" t="s">
+        <v>122</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="60"/>

</xml_diff>

<commit_message>
Changed the browser type and updated code for remit
</commit_message>
<xml_diff>
--- a/ExcelSheets/REMIT/TC_Remit.xlsx
+++ b/ExcelSheets/REMIT/TC_Remit.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="133">
   <si>
     <t xml:space="preserve">TCID</t>
   </si>
@@ -45,6 +45,9 @@
     <t xml:space="preserve">Validate the user Login into the System</t>
   </si>
   <si>
+    <t xml:space="preserve">Fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_AddNewSender</t>
   </si>
   <si>
@@ -54,6 +57,9 @@
     <t xml:space="preserve">Validate a New Sender can be added</t>
   </si>
   <si>
+    <t xml:space="preserve">Skip</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_ExistingSender</t>
   </si>
   <si>
@@ -159,123 +165,105 @@
     <t xml:space="preserve">Expected text</t>
   </si>
   <si>
+    <t xml:space="preserve">GetText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Userbal_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closeBrowser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getLogin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO Otp Panel Displayed FAILPASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text is not verified FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_searchNumber_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add/Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existName_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully Fetched the value PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existBalance_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">takeScreenShot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addSender_Name_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SenderName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addOtpNumber_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addSenderConfirmBtn_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beneficaryAddBtn_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchBank_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BankName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icicBnk_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beneficiaryAccountNum_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccountNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beneficiaryPhoneNum_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhoneNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addBeneficiaryBtn_xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Text is verified PASS</t>
   </si>
   <si>
-    <t xml:space="preserve">GetText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Userbal_xpath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Successfully Fetched the value PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closeBrowser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">getLogin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add_searchNumber_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add/Search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existName_xpath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existBalance_xpath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">takeScreenShot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INFO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addSender_Name_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SenderName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addOtpNumber_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addSenderConfirmBtn_xpath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO Otp Panel Displayed FAILPASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waited for 20 sec PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beneficaryAddBtn_xpath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clicked on beneficaryAddBtn_xpath PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchBank_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BankName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">icicBnk_xpath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clicked on icicBnk_xpath PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beneficiaryAccountNum_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AccountNum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beneficiaryPhoneNum_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PhoneNo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addBeneficiaryBtn_xpath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clicked on addBeneficiaryBtn_xpath PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unable to take the screenshot FAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Text is not verified FAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error While entering the Values ERROR</t>
-  </si>
-  <si>
     <t xml:space="preserve">firstradio_xpath</t>
   </si>
   <si>
@@ -315,7 +303,7 @@
     <t xml:space="preserve">Actual Result</t>
   </si>
   <si>
-    <t xml:space="preserve">Chrome</t>
+    <t xml:space="preserve">Mozilla</t>
   </si>
   <si>
     <t xml:space="preserve">9819042543</t>
@@ -327,12 +315,6 @@
     <t xml:space="preserve">Test Anand 123</t>
   </si>
   <si>
-    <t xml:space="preserve">Test got Successfully Passed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass</t>
-  </si>
-  <si>
     <t xml:space="preserve">ExpectedResult</t>
   </si>
   <si>
@@ -354,7 +336,10 @@
     <t xml:space="preserve">100</t>
   </si>
   <si>
-    <t>Successfully created a instance of chrome PASS</t>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>Successfully created a instance of Mozilla PASS</t>
   </si>
   <si>
     <t>Successfully navigated to Live_url PASS</t>
@@ -363,13 +348,52 @@
     <t>NO Otp Panel Displayed FAILPASS</t>
   </si>
   <si>
+    <t>Text is verified PASS</t>
+  </si>
+  <si>
+    <t>Successfully Fetched the value PASS</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Entered Value in the Field PASS</t>
+  </si>
+  <si>
     <t>Waited for 20 sec PASS</t>
   </si>
   <si>
-    <t>Text is verified PASS</t>
-  </si>
-  <si>
-    <t>Entered Value in the Field PASS</t>
+    <t>Clicked on beneficaryAddBtn_xpath PASS</t>
+  </si>
+  <si>
+    <t>Clicked on icicBnk_xpath PASS</t>
+  </si>
+  <si>
+    <t>Clicked on addBeneficiaryBtn_xpath PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Failed to excute the test</t>
+  </si>
+  <si>
+    <t>Error While entering the Values ERROR</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Test got Successfully Passed</t>
+  </si>
+  <si>
+    <t>Clicked on loginButton_xpath PASS</t>
+  </si>
+  <si>
+    <t>NO Otp Panel Displayed FAIL</t>
   </si>
   <si>
     <t>Clicked on firstradio_xpath PASS</t>
@@ -378,42 +402,6 @@
     <t>Clicked on transferBtn_id PASS</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Test got Successfully Passed</t>
-  </si>
-  <si>
-    <t>Skip</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Error While entering the Values ERROR</t>
-  </si>
-  <si>
-    <t>Clicked on loginButton_xpath PASS</t>
-  </si>
-  <si>
-    <t>NO Otp Panel Displayed FAIL</t>
-  </si>
-  <si>
-    <t>Successfully Fetched the value PASS</t>
-  </si>
-  <si>
-    <t>Clicked on beneficaryAddBtn_xpath PASS</t>
-  </si>
-  <si>
-    <t>Clicked on icicBnk_xpath PASS</t>
-  </si>
-  <si>
-    <t>Clicked on addBeneficiaryBtn_xpath PASS</t>
-  </si>
-  <si>
     <t>Successfully navigated to report_url PASS</t>
   </si>
   <si>
@@ -424,6 +412,12 @@
   </si>
   <si>
     <t>Accepting the Alert Option PASS</t>
+  </si>
+  <si>
+    <t>NO Otp Panel Displayed PASSPASS</t>
+  </si>
+  <si>
+    <t>NO Otp Panel Displayed PASS</t>
   </si>
   <si>
     <t>Text is not verified FAIL</t>
@@ -581,7 +575,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="280">
+  <cellXfs count="351">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -598,38 +592,38 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -685,6 +679,219 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="true"/>
@@ -1528,16 +1735,16 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D2" activeCellId="0" pane="topLeft" sqref="D2"/>
+      <selection activeCell="D2" activeCellId="13" pane="topLeft" sqref="G3 G13 G18 G23 G27 G32 G37:H37 I13 I23 I27 I32 L18 H3 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="1" width="24.8367346938776" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="1" width="49.1377551020408" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="1" width="24.3010204081633" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="1" width="10.6632653061225" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="1" width="47.9234693877551" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" hidden="false" style="1" width="7.60546875" collapsed="true"/>
-    <col min="5" max="1025" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
+    <col min="5" max="1025" hidden="false" style="1" width="10.6632653061225" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="1">
@@ -1564,106 +1771,106 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="241" t="s">
-        <v>122</v>
+      <c r="D2" s="315" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="3">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="270" t="s">
-        <v>121</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="266" t="s">
+        <v>104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="4">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="227" t="s">
-        <v>122</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="300" t="s">
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="5">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="277" t="s">
-        <v>122</v>
+        <v>15</v>
+      </c>
+      <c r="D5" s="289" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="246" t="s">
-        <v>122</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="331" t="s">
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="7">
       <c r="A7" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="232" t="s">
-        <v>122</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="305" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="8">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="251" t="s">
-        <v>122</v>
+        <v>21</v>
+      </c>
+      <c r="D8" s="336" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="9">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="256" t="s">
-        <v>122</v>
+        <v>23</v>
+      </c>
+      <c r="D9" s="350" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1682,20 +1889,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D103" activeCellId="0" pane="topLeft" sqref="D103"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B14" activeCellId="13" pane="topLeft" sqref="G3 G13 G18 G23 G27 G32 G37:H37 I13 I23 I27 I32 L18 H3 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="7" width="31.7244897959184" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="7" width="22.0051020408163" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="7" width="31.0459183673469" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="7" width="21.0612244897959" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" hidden="false" style="7" width="41.0546875" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="7" width="11.0714285714286" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="7" width="30.9132653061224" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="7" width="21.4642857142857" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="7" width="30.2397959183673" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="7" width="20.3826530612245" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" hidden="false" style="7" width="40.46875" collapsed="true"/>
+    <col min="6" max="1025" hidden="false" style="7" width="10.6632653061225" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="1">
@@ -1703,13 +1910,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>3</v>
@@ -1720,14 +1927,14 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="233" t="s">
-        <v>110</v>
+        <v>28</v>
+      </c>
+      <c r="E2" s="306" t="s">
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="3">
@@ -1735,14 +1942,14 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="9"/>
-      <c r="E3" s="234" t="s">
-        <v>111</v>
+      <c r="E3" s="307" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="4">
@@ -1750,16 +1957,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="235" t="s">
-        <v>115</v>
+        <v>35</v>
+      </c>
+      <c r="E4" s="308" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="5">
@@ -1767,16 +1974,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="236" t="s">
-        <v>115</v>
+        <v>38</v>
+      </c>
+      <c r="E5" s="309" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
@@ -1784,14 +1991,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="237" t="s">
-        <v>124</v>
+      <c r="E6" s="310" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="7">
@@ -1799,12 +2006,12 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="238" t="s">
-        <v>125</v>
+      <c r="E7" s="311" t="s">
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="8">
@@ -1812,16 +2019,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="E8" s="312" t="s">
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="9">
@@ -1829,15 +2036,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="E9" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="10">
       <c r="A10" s="6" t="s">
@@ -1848,1290 +2053,1321 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="E10" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="11">
-      <c r="A11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="278" t="s">
-        <v>110</v>
-      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="12">
       <c r="A12" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="279" t="s">
-        <v>111</v>
+      <c r="E12" s="290" t="s">
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="13">
       <c r="A13" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="148" t="s">
-        <v>112</v>
+      <c r="E13" s="291" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="14">
       <c r="A14" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="149" t="s">
-        <v>114</v>
+        <v>50</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="292" t="s">
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="15">
       <c r="A15" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="150" t="s">
-        <v>115</v>
+        <v>45</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="293" t="s">
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="16">
       <c r="A16" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="151" t="s">
-        <v>126</v>
+      <c r="E16" s="294" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="17">
       <c r="A17" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="152" t="s">
-        <v>126</v>
+      <c r="E17" s="295" t="s">
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
       <c r="A18" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="296" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="19">
       <c r="A19" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="20">
+      <c r="A20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="153" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="20">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="13"/>
+      <c r="E20" s="297" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
-      <c r="A21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="D21" s="9"/>
       <c r="E21" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="9"/>
       <c r="E22" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="23">
       <c r="A23" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="24">
       <c r="A24" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>44</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="25">
       <c r="A25" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="E25" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="26">
       <c r="A26" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>53</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D26" s="9"/>
       <c r="E26" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="27">
       <c r="A27" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E27" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="28">
       <c r="A28" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>61</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D28" s="9"/>
       <c r="E28" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="29">
       <c r="A29" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="9"/>
+      <c r="D29" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="E29" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="30">
       <c r="A30" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="31">
       <c r="A31" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="32">
       <c r="A32" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="33">
       <c r="A33" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="34">
       <c r="A34" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="6"/>
+        <v>58</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="D34" s="9"/>
       <c r="E34" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="35">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
+      <c r="A35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="C35" s="6"/>
       <c r="D35" s="9"/>
       <c r="E35" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="36">
-      <c r="A36" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="271" t="s">
-        <v>110</v>
-      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="37">
       <c r="A37" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="272" t="s">
-        <v>111</v>
+      <c r="E37" s="267" t="s">
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="38">
       <c r="A38" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="D38" s="9"/>
-      <c r="E38" s="273" t="s">
-        <v>112</v>
+      <c r="E38" s="268" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="39">
       <c r="A39" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="274" t="s">
-        <v>134</v>
+        <v>50</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="269" t="s">
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="40">
       <c r="A40" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B40" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="127" t="s">
-        <v>126</v>
+      <c r="E40" s="270" t="s">
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="41">
       <c r="A41" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D41" s="9"/>
-      <c r="E41" s="128" t="s">
-        <v>118</v>
+      <c r="E41" s="271" t="s">
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="42">
       <c r="A42" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="129" t="s">
-        <v>115</v>
+        <v>60</v>
+      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="272" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="43">
       <c r="A43" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="130" t="s">
-        <v>113</v>
+        <v>53</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="273" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="44">
       <c r="A44" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D44" s="9"/>
-      <c r="E44" s="131" t="s">
-        <v>126</v>
+      <c r="E44" s="274" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="45">
       <c r="A45" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D45" s="9"/>
-      <c r="E45" s="132" t="s">
-        <v>126</v>
+      <c r="E45" s="275" t="s">
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="46">
       <c r="A46" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D46" s="9"/>
-      <c r="E46" s="13"/>
+      <c r="E46" s="276" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="47">
       <c r="A47" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D47" s="9"/>
-      <c r="E47" s="133" t="s">
-        <v>127</v>
-      </c>
+      <c r="E47" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="48">
       <c r="A48" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D48" s="9"/>
-      <c r="E48" s="134" t="s">
+      <c r="E48" s="277" t="s">
         <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="49">
       <c r="A49" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="135" t="s">
-        <v>115</v>
+        <v>68</v>
+      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" s="278" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="50">
       <c r="A50" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="136" t="s">
-        <v>128</v>
+        <v>70</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" s="279" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="51">
       <c r="A51" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D51" s="9"/>
-      <c r="E51" s="137" t="s">
-        <v>113</v>
+      <c r="E51" s="280" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="52">
       <c r="A52" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" s="138" t="s">
-        <v>115</v>
+        <v>62</v>
+      </c>
+      <c r="D52" s="9"/>
+      <c r="E52" s="281" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="53">
       <c r="A53" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E53" s="139" t="s">
-        <v>115</v>
+        <v>74</v>
+      </c>
+      <c r="E53" s="282" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="54">
       <c r="A54" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="140" t="s">
-        <v>129</v>
+        <v>75</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54" s="283" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="55">
       <c r="A55" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D55" s="6"/>
-      <c r="E55" s="141" t="s">
-        <v>113</v>
+      <c r="E55" s="284" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="56">
       <c r="A56" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="D56" s="6"/>
-      <c r="E56" s="4" t="s">
-        <v>81</v>
+      <c r="E56" s="285" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="57">
       <c r="A57" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C57" s="6"/>
+        <v>58</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="D57" s="6"/>
-      <c r="E57" s="142" t="s">
-        <v>118</v>
-      </c>
+      <c r="E57" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="58">
       <c r="A58" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C58" s="6"/>
-      <c r="D58" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E58" s="228" t="s">
-        <v>110</v>
+      <c r="D58" s="6"/>
+      <c r="E58" s="286" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="59">
-      <c r="A59" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
       <c r="D59" s="6"/>
-      <c r="E59" s="229" t="s">
-        <v>111</v>
-      </c>
+      <c r="E59" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="60">
       <c r="A60" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="159" t="s">
-        <v>112</v>
+      <c r="D60" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" s="301" t="s">
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="61">
       <c r="A61" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E61" s="160" t="s">
-        <v>114</v>
+        <v>31</v>
+      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="302" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="62">
       <c r="A62" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E62" s="161" t="s">
-        <v>115</v>
+        <v>50</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="208" t="s">
+        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="63">
       <c r="A63" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B63" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C63" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="162" t="s">
-        <v>126</v>
+      <c r="E63" s="209" t="s">
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="64">
       <c r="A64" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="163" t="s">
-        <v>126</v>
+        <v>53</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E64" s="210" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="65">
       <c r="A65" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D65" s="6"/>
-      <c r="E65" s="13"/>
+      <c r="E65" s="211" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="66">
       <c r="A66" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B66" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D66" s="6"/>
+      <c r="E66" s="212" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="67">
+      <c r="A67" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="6"/>
+      <c r="E67" s="13"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="68">
+      <c r="A68" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="164" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="67">
-      <c r="A67" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E67" s="242" t="s">
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="213" t="s">
         <v>110</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="68">
-      <c r="A68" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D68" s="9"/>
-      <c r="E68" s="243" t="s">
-        <v>111</v>
-      </c>
-    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="69">
-      <c r="A69" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
       <c r="C69" s="6"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="179" t="s">
-        <v>112</v>
-      </c>
+      <c r="D69" s="6"/>
+      <c r="E69" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="70">
       <c r="A70" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D70" s="9"/>
-      <c r="E70" s="180" t="s">
-        <v>113</v>
+        <v>27</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" s="316" t="s">
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="71">
       <c r="A71" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E71" s="181" t="s">
-        <v>114</v>
+        <v>31</v>
+      </c>
+      <c r="D71" s="9"/>
+      <c r="E71" s="317" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="72">
       <c r="A72" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D72" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="318" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="73">
+      <c r="A73" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D73" s="9"/>
+      <c r="E73" s="319" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="74">
+      <c r="A74" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E74" s="320" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="75">
+      <c r="A75" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E72" s="182" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="73">
-      <c r="A73" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D73" s="6"/>
-      <c r="E73" s="183" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="74">
-      <c r="A74" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E74" s="184" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="75">
-      <c r="A75" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D75" s="6"/>
-      <c r="E75" s="185" t="s">
-        <v>113</v>
+      <c r="D75" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E75" s="321" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="76">
       <c r="A76" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="D76" s="6"/>
-      <c r="E76" s="13"/>
+      <c r="E76" s="322" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="77">
       <c r="A77" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D77" s="6"/>
-      <c r="E77" s="186" t="s">
-        <v>117</v>
+        <v>81</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E77" s="323" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="78">
       <c r="A78" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="D78" s="6"/>
-      <c r="E78" s="187" t="s">
-        <v>113</v>
+      <c r="E78" s="324" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="79">
       <c r="A79" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D79" s="6"/>
-      <c r="E79" s="188" t="s">
-        <v>118</v>
-      </c>
+      <c r="E79" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="80">
       <c r="A80" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B80" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D80" s="6"/>
+      <c r="E80" s="325" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="81">
+      <c r="A81" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" s="6"/>
+      <c r="E81" s="326" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="82">
+      <c r="A82" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D82" s="6"/>
+      <c r="E82" s="327" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="83">
+      <c r="A83" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="189" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="81">
-      <c r="A81" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E81" s="247" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="82">
-      <c r="A82" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D82" s="9"/>
-      <c r="E82" s="248" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="83">
-      <c r="A83" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
-      <c r="E83" s="195" t="s">
-        <v>112</v>
+      <c r="E83" s="328" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="84">
-      <c r="A84" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E84" s="196" t="s">
-        <v>114</v>
-      </c>
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="85">
       <c r="A85" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B85" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C85" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D85" s="6"/>
-      <c r="E85" s="197" t="s">
-        <v>130</v>
+      <c r="E85" s="332" t="s">
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="86">
       <c r="A86" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E86" s="198" t="s">
-        <v>114</v>
+        <v>31</v>
+      </c>
+      <c r="D86" s="9"/>
+      <c r="E86" s="333" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="87">
       <c r="A87" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C87" s="6"/>
       <c r="D87" s="6"/>
-      <c r="E87" s="13"/>
+      <c r="E87" s="244" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="88">
       <c r="A88" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B88" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E88" s="245" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="89">
+      <c r="A89" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D89" s="6"/>
+      <c r="E89" s="246" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="90">
+      <c r="A90" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E90" s="247" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="91">
+      <c r="A91" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D91" s="6"/>
+      <c r="E91" s="13"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="92">
+      <c r="A92" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="199" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="89">
-      <c r="A89" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C89" s="6"/>
-      <c r="D89" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E89" s="252" t="s">
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="248" t="s">
         <v>110</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="90">
-      <c r="A90" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D90" s="9"/>
-      <c r="E90" s="253" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="91">
-      <c r="A91" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="205" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="92">
-      <c r="A92" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E92" s="206" t="s">
-        <v>114</v>
-      </c>
-    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="93">
-      <c r="A93" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E93" s="207" t="s">
-        <v>115</v>
-      </c>
+      <c r="A93" s="3"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="94">
       <c r="A94" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E94" s="208" t="s">
-        <v>116</v>
+        <v>22</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C94" s="6"/>
+      <c r="D94" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" s="337" t="s">
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="95">
       <c r="A95" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E95" s="209" t="s">
-        <v>131</v>
+        <v>22</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D95" s="9"/>
+      <c r="E95" s="338" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="96">
       <c r="A96" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E96" s="210" t="s">
-        <v>113</v>
+        <v>50</v>
+      </c>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="339" t="s">
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="97">
       <c r="A97" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C97" s="0"/>
-      <c r="E97" s="211" t="s">
-        <v>132</v>
+        <v>22</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E97" s="340" t="s">
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="98">
       <c r="A98" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E98" s="212" t="s">
-        <v>133</v>
+        <v>22</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E98" s="341" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="99">
       <c r="A99" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B99" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E99" s="342" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="100">
+      <c r="A100" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E100" s="343" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="101">
+      <c r="A101" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E101" s="344" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="102">
+      <c r="A102" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C102" s="0"/>
+      <c r="E102" s="345" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="103">
+      <c r="A103" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E103" s="346" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="104">
+      <c r="A104" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E99" s="213" t="s">
-        <v>118</v>
+      <c r="E104" s="347" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3152,25 +3388,25 @@
   </sheetPr>
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I13" activeCellId="0" pane="topLeft" sqref="I13"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H3" activeCellId="12" pane="topLeft" sqref="G3 G13 G18 G23 G27 G32 G37:H37 I13 I23 I27 I32 L18 H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="1" width="27.1326530612245" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="1" width="13.6326530612245" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="1" width="22.2755102040816" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="1" width="19.7091836734694" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" hidden="false" style="1" width="15.33203125" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="1" width="26.3214285714286" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="1" width="10.6632653061225" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="1" width="13.2295918367347" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="1" width="10.6632653061225" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="1" width="21.734693877551" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="1" width="19.1683673469388" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" hidden="false" style="1" width="24.9453125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" hidden="false" style="1" width="12.01953125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" hidden="false" style="1" width="12.01953125" collapsed="true"/>
-    <col min="10" max="10" hidden="false" style="1" width="13.7704081632653" collapsed="true"/>
-    <col min="11" max="11" hidden="false" style="1" width="13.6326530612245" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="1" width="17.5051020408163" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="1" width="13.2295918367347" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" hidden="false" style="1" width="6.171875" collapsed="true"/>
-    <col min="13" max="1025" hidden="false" style="1" width="11.0714285714286" collapsed="true"/>
+    <col min="13" max="1025" hidden="false" style="1" width="10.6632653061225" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="1">
@@ -3194,22 +3430,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>3</v>
@@ -3224,21 +3460,23 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="240"/>
-      <c r="H3" s="239" t="s">
-        <v>122</v>
+      <c r="G3" s="314" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="313" t="s">
+        <v>117</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="10"/>
@@ -3275,7 +3513,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
       <c r="A6" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -3294,28 +3532,28 @@
         <v>1</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J7" s="21" t="s">
         <v>3</v>
@@ -3328,24 +3566,24 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="13"/>
       <c r="H8" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="10"/>
@@ -3381,7 +3619,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="11">
       <c r="A11" s="16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -3400,25 +3638,25 @@
         <v>1</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I12" s="21" t="s">
         <v>3</v>
@@ -3432,24 +3670,26 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="299" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="226"/>
-      <c r="H13" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I13" s="225" t="s">
-        <v>122</v>
+      <c r="I13" s="298" t="s">
+        <v>120</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -3485,7 +3725,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="16">
       <c r="A16" s="16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -3504,34 +3744,34 @@
         <v>1</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H17" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I17" s="23" t="s">
         <v>71</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L17" s="21" t="s">
         <v>3</v>
@@ -3542,33 +3782,35 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E18" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="0"/>
+      <c r="G18" s="288" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="0"/>
-      <c r="G18" s="276"/>
-      <c r="H18" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="I18" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L18" s="275" t="s">
-        <v>122</v>
+        <v>100</v>
+      </c>
+      <c r="L18" s="287" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="19">
@@ -3599,7 +3841,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
       <c r="A21" s="24" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
@@ -3617,31 +3859,31 @@
         <v>1</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I22" s="21" t="s">
         <v>3</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K22" s="23"/>
     </row>
@@ -3650,27 +3892,29 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E23" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="0"/>
+      <c r="G23" s="330" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F23" s="0"/>
-      <c r="G23" s="245"/>
-      <c r="H23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I23" s="244" t="s">
-        <v>122</v>
+      <c r="I23" s="329" t="s">
+        <v>120</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="24">
@@ -3687,7 +3931,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="25">
       <c r="A25" s="25" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B25" s="0"/>
       <c r="C25" s="0"/>
@@ -3704,25 +3948,25 @@
         <v>1</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>3</v>
@@ -3734,24 +3978,26 @@
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E27" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="304" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="231"/>
-      <c r="H27" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I27" s="230" t="s">
-        <v>122</v>
+      <c r="I27" s="303" t="s">
+        <v>117</v>
       </c>
       <c r="J27" s="0"/>
     </row>
@@ -3781,7 +4027,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="30">
       <c r="A30" s="16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B30" s="0"/>
       <c r="C30" s="0"/>
@@ -3798,31 +4044,31 @@
         <v>1</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H31" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>3</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="32">
@@ -3830,30 +4076,32 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E32" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="335" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="250"/>
-      <c r="H32" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I32" s="249" t="s">
-        <v>122</v>
+      <c r="I32" s="334" t="s">
+        <v>117</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="33">
+        <v>102</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="33">
       <c r="A33" s="0"/>
       <c r="B33" s="0"/>
       <c r="C33" s="0"/>
@@ -3864,7 +4112,7 @@
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="34">
       <c r="A34" s="0"/>
       <c r="B34" s="0"/>
       <c r="C34" s="0"/>
@@ -3877,7 +4125,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="35">
       <c r="A35" s="25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B35" s="0"/>
       <c r="C35" s="0"/>
@@ -3893,28 +4141,28 @@
         <v>1</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H36" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="37">
@@ -3922,24 +4170,26 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E37" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="349" t="s">
+        <v>121</v>
+      </c>
+      <c r="H37" s="348" t="s">
+        <v>120</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="255"/>
-      <c r="H37" s="254" t="s">
-        <v>122</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="60"/>

</xml_diff>